<commit_message>
refactored apart from heatmaps
</commit_message>
<xml_diff>
--- a/vis/people_sheet.xlsx
+++ b/vis/people_sheet.xlsx
@@ -295,19 +295,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2A5DA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBE7EC7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBD93A1"/>
+        <fgColor rgb="FF9D93FE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF9C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF79AD92"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,181 +319,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF185EE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF47F88"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFEF8D0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC1DCDE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9DDFB2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6C7FB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA7AEFA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5A47C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB5CB81"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFECE87B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7CC8FD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8FC593"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDBB0A7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB5FD8B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF79FCA0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7F80E0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF0F3F8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBD7AF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB5F3FE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8B3C2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF83F9EB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7AAF7E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA28B8B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF695B6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB688ED"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92EA79"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808CA9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFACFCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF82BABF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD0EEB8"/>
+        <fgColor rgb="FFD57EF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6D7EC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBDB93"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7AE3D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBC0DE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A8C5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2ACB6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCD289"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBEDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF847F7F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2A0FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BE586"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF837AEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7FD99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDF5F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA88AA5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1AB9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4C9CB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0FA7C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF67EBC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7C97CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2848D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF8CD1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF96FABF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFB580"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA927C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB9BDF2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF88C9BA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91DAF5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF894D6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>